<commit_message>
do aeon's ergo buffnerf and move weight from the bcg
</commit_message>
<xml_diff>
--- a/changes/aug-barrels.xlsx
+++ b/changes/aug-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2896E8-5904-41A2-B6C1-0A915AEB2B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DF100A-B377-4C04-AFDC-3033A14A3C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>new</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Steyr AUG HBAR 5.56x45 620mm Heavy LMG</t>
+  </si>
+  <si>
+    <t>aug_a3_std_bolt_carrier</t>
+  </si>
+  <si>
+    <t>AUG A3 Std.</t>
   </si>
 </sst>
 </file>
@@ -942,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,10 +1016,10 @@
         <v>20</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>0.39</v>
+        <v>0.54</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1035,7 +1041,7 @@
       </c>
       <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*5+J3/300</f>
-        <v>-4.6666666666666679</v>
+        <v>-13.666666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1046,10 +1052,10 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.48</v>
+        <v>0.63</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1071,7 +1077,7 @@
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N6" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*5+J4/300</f>
-        <v>-3.6333333333333333</v>
+        <v>-12.633333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1082,10 +1088,10 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="D5">
-        <v>0.59</v>
+        <v>0.79</v>
       </c>
       <c r="E5">
         <v>-2</v>
@@ -1107,7 +1113,7 @@
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>-3.5333333333333323</v>
+        <v>-12.533333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1118,10 +1124,10 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <v>-7</v>
+        <v>-12</v>
       </c>
       <c r="D6">
-        <v>0.8</v>
+        <v>0.98</v>
       </c>
       <c r="E6">
         <v>-5</v>
@@ -1143,7 +1149,24 @@
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>-12.200000000000001</v>
+        <v>-20.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>